<commit_message>
list multiCompnay name here
</commit_message>
<xml_diff>
--- a/StockMarket01_log.xlsx
+++ b/StockMarket01_log.xlsx
@@ -405,303 +405,4 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Timestamp</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Company</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Ticker</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Open</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Close</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Matched</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-05-15 15:27:10</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Reliance Industries Limited</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>RELIANCE.NS</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1454.5</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1454.5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1454.5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1454.5</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-05-15 15:32:19</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Reliance Industries Limited</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>RELIANCE.NS</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1453.300048828125</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1452.900024414062</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1454.599975585938</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1453</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-05-15 15:37:24</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Reliance Industries Limited</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>RELIANCE.NS</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1453.300048828125</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1452.900024414062</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1454.599975585938</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1453</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-05-15 15:42:29</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Reliance Industries Limited</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>RELIANCE.NS</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>1453.300048828125</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1452.900024414062</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1454.599975585938</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1453</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-05-15 15:46:51</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Reliance Industries Limited</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>RELIANCE.NS</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1453.300048828125</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1452.900024414062</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1454.599975585938</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1453</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-05-15 15:51:52</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Reliance Industries Limited</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>RELIANCE.NS</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1453.300048828125</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1452.900024414062</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1454.599975585938</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1453</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-05-15 16:08:50</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Reliance Industries Limited</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>RELIANCE.NS</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1455.699951171875</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1452.900024414062</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1455.900024414062</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1453</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>